<commit_message>
ajout de la TVA ^^
</commit_message>
<xml_diff>
--- a/electronique/liste des courses.xlsx
+++ b/electronique/liste des courses.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
   <si>
     <t>ref RS</t>
   </si>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t>Total des dépenses :</t>
+  </si>
+  <si>
+    <t>Prix HT :</t>
   </si>
 </sst>
 </file>
@@ -257,19 +260,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,7 +556,7 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -592,14 +595,14 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C4" s="1" t="s">
@@ -636,7 +639,7 @@
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C5" t="s">
@@ -674,7 +677,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
+      <c r="A6" s="9"/>
       <c r="C6" t="s">
         <v>9</v>
       </c>
@@ -710,7 +713,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
+      <c r="A7" s="9"/>
       <c r="C7" t="s">
         <v>25</v>
       </c>
@@ -746,7 +749,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
+      <c r="A8" s="9"/>
       <c r="B8" t="s">
         <v>21</v>
       </c>
@@ -785,7 +788,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
+      <c r="A9" s="9"/>
       <c r="C9" t="s">
         <v>12</v>
       </c>
@@ -821,7 +824,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
+      <c r="A10" s="9"/>
       <c r="C10" t="s">
         <v>13</v>
       </c>
@@ -857,7 +860,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="9" t="s">
         <v>27</v>
       </c>
       <c r="C11" t="s">
@@ -895,7 +898,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
+      <c r="A12" s="9"/>
       <c r="C12" t="s">
         <v>24</v>
       </c>
@@ -931,7 +934,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
+      <c r="A13" s="9"/>
       <c r="B13" t="s">
         <v>21</v>
       </c>
@@ -970,7 +973,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
+      <c r="A14" s="9"/>
       <c r="C14" t="s">
         <v>24</v>
       </c>
@@ -1006,7 +1009,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
+      <c r="A15" s="9"/>
       <c r="C15" t="s">
         <v>24</v>
       </c>
@@ -1042,7 +1045,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
+      <c r="A16" s="9"/>
       <c r="C16" t="s">
         <v>44</v>
       </c>
@@ -1078,7 +1081,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
+      <c r="A17" s="9"/>
       <c r="C17" t="s">
         <v>43</v>
       </c>
@@ -1114,7 +1117,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
+      <c r="A18" s="9"/>
       <c r="C18" t="s">
         <v>45</v>
       </c>
@@ -1150,7 +1153,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C19" t="s">
@@ -1188,7 +1191,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
+      <c r="A20" s="7"/>
       <c r="C20" t="s">
         <v>24</v>
       </c>
@@ -1224,7 +1227,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C21" t="s">
@@ -1262,7 +1265,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
+      <c r="A22" s="7"/>
       <c r="C22" t="s">
         <v>47</v>
       </c>
@@ -1298,7 +1301,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
+      <c r="A23" s="7"/>
       <c r="C23" t="s">
         <v>48</v>
       </c>
@@ -1334,7 +1337,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
+      <c r="A24" s="7"/>
       <c r="C24" t="s">
         <v>49</v>
       </c>
@@ -1370,12 +1373,21 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="K26" s="6" t="s">
-        <v>56</v>
+      <c r="K26" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="L26">
         <f>SUM(L5:L24)</f>
         <v>58.605999999999995</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K27" t="s">
+        <v>56</v>
+      </c>
+      <c r="L27">
+        <f>L26*1.2</f>
+        <v>70.327199999999991</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
@@ -1420,28 +1432,28 @@
       </c>
     </row>
     <row r="33" spans="11:14" x14ac:dyDescent="0.3">
-      <c r="K33" s="9" t="s">
+      <c r="K33" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="L33" s="9"/>
-      <c r="M33" s="9"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
       <c r="N33">
-        <f>L26+N28+N31</f>
-        <v>259.12599999999998</v>
+        <f>L27+N28+N31</f>
+        <v>270.84719999999999</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="A5:A10"/>
+    <mergeCell ref="A11:A18"/>
+    <mergeCell ref="A19:A20"/>
     <mergeCell ref="K33:M33"/>
     <mergeCell ref="A21:A24"/>
     <mergeCell ref="K28:M28"/>
     <mergeCell ref="K29:M29"/>
     <mergeCell ref="K30:M30"/>
     <mergeCell ref="K31:M31"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="A5:A10"/>
-    <mergeCell ref="A11:A18"/>
-    <mergeCell ref="A19:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
maj liste des composants
</commit_message>
<xml_diff>
--- a/electronique/liste des courses.xlsx
+++ b/electronique/liste des courses.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="72">
   <si>
     <t>ref RS</t>
   </si>
@@ -213,6 +213,33 @@
   </si>
   <si>
     <t>Prix HT :</t>
+  </si>
+  <si>
+    <t>Condensateur</t>
+  </si>
+  <si>
+    <t>721-5240</t>
+  </si>
+  <si>
+    <t>100nF</t>
+  </si>
+  <si>
+    <t>335-000</t>
+  </si>
+  <si>
+    <t>1,5µF</t>
+  </si>
+  <si>
+    <t>2,2nF</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>1K2</t>
+  </si>
+  <si>
+    <t>1M</t>
   </si>
 </sst>
 </file>
@@ -248,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -268,10 +295,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -555,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O33" sqref="O33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -639,7 +667,7 @@
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C5" t="s">
@@ -677,7 +705,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
+      <c r="A6" s="8"/>
       <c r="C6" t="s">
         <v>9</v>
       </c>
@@ -713,7 +741,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
+      <c r="A7" s="8"/>
       <c r="C7" t="s">
         <v>25</v>
       </c>
@@ -749,7 +777,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
+      <c r="A8" s="8"/>
       <c r="B8" t="s">
         <v>21</v>
       </c>
@@ -788,7 +816,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
+      <c r="A9" s="8"/>
       <c r="C9" t="s">
         <v>12</v>
       </c>
@@ -824,7 +852,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
+      <c r="A10" s="8"/>
       <c r="C10" t="s">
         <v>13</v>
       </c>
@@ -860,7 +888,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C11" t="s">
@@ -898,7 +926,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="9"/>
+      <c r="A12" s="8"/>
       <c r="C12" t="s">
         <v>24</v>
       </c>
@@ -934,7 +962,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="9"/>
+      <c r="A13" s="8"/>
       <c r="B13" t="s">
         <v>21</v>
       </c>
@@ -973,7 +1001,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
+      <c r="A14" s="8"/>
       <c r="C14" t="s">
         <v>24</v>
       </c>
@@ -1009,7 +1037,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
+      <c r="A15" s="8"/>
       <c r="C15" t="s">
         <v>24</v>
       </c>
@@ -1045,7 +1073,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
+      <c r="A16" s="8"/>
       <c r="C16" t="s">
         <v>44</v>
       </c>
@@ -1081,7 +1109,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="9"/>
+      <c r="A17" s="8"/>
       <c r="C17" t="s">
         <v>43</v>
       </c>
@@ -1117,7 +1145,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="9"/>
+      <c r="A18" s="8"/>
       <c r="C18" t="s">
         <v>45</v>
       </c>
@@ -1372,7 +1400,31 @@
         <v>5.6999999999999993</v>
       </c>
     </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" t="s">
+        <v>65</v>
+      </c>
+      <c r="F25" t="s">
+        <v>69</v>
+      </c>
+    </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" s="7"/>
+      <c r="C26" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
       <c r="K26" s="4" t="s">
         <v>62</v>
       </c>
@@ -1382,6 +1434,13 @@
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" s="7"/>
+      <c r="D27" t="s">
+        <v>68</v>
+      </c>
+      <c r="F27">
+        <v>3</v>
+      </c>
       <c r="K27" t="s">
         <v>56</v>
       </c>
@@ -1391,59 +1450,71 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="K28" s="8" t="s">
+      <c r="D28" t="s">
+        <v>70</v>
+      </c>
+      <c r="F28">
+        <v>3</v>
+      </c>
+      <c r="K28" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
       <c r="N28">
         <v>76.52</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="K29" s="8" t="s">
+      <c r="D29" t="s">
+        <v>71</v>
+      </c>
+      <c r="F29">
+        <v>2</v>
+      </c>
+      <c r="K29" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
       <c r="N29">
         <v>174</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="K30" s="8" t="s">
+      <c r="K30" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
       <c r="N30">
         <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="K31" s="8" t="s">
+      <c r="K31" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
       <c r="N31">
         <f>N29-N30</f>
         <v>124</v>
       </c>
     </row>
     <row r="33" spans="11:14" x14ac:dyDescent="0.3">
-      <c r="K33" s="6" t="s">
+      <c r="K33" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
       <c r="N33">
         <f>L27+N28+N31</f>
         <v>270.84719999999999</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="A5:A10"/>
     <mergeCell ref="A11:A18"/>
@@ -1454,6 +1525,7 @@
     <mergeCell ref="K29:M29"/>
     <mergeCell ref="K30:M30"/>
     <mergeCell ref="K31:M31"/>
+    <mergeCell ref="A25:A27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Ajout doc + mise a jour des modeles 3D
</commit_message>
<xml_diff>
--- a/electronique/liste des courses.xlsx
+++ b/electronique/liste des courses.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="75">
   <si>
     <t>ref RS</t>
   </si>
@@ -240,6 +240,15 @@
   </si>
   <si>
     <t>1M</t>
+  </si>
+  <si>
+    <t>877-3444</t>
+  </si>
+  <si>
+    <t>148-528</t>
+  </si>
+  <si>
+    <t>133-217</t>
   </si>
 </sst>
 </file>
@@ -275,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -290,6 +299,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -583,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -623,11 +633,11 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
@@ -667,7 +677,7 @@
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C5" t="s">
@@ -705,7 +715,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
+      <c r="A6" s="9"/>
       <c r="C6" t="s">
         <v>9</v>
       </c>
@@ -741,7 +751,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
+      <c r="A7" s="9"/>
       <c r="C7" t="s">
         <v>25</v>
       </c>
@@ -777,7 +787,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
+      <c r="A8" s="9"/>
       <c r="B8" t="s">
         <v>21</v>
       </c>
@@ -816,7 +826,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
+      <c r="A9" s="9"/>
       <c r="C9" t="s">
         <v>12</v>
       </c>
@@ -852,7 +862,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
+      <c r="A10" s="9"/>
       <c r="C10" t="s">
         <v>13</v>
       </c>
@@ -888,7 +898,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="9" t="s">
         <v>27</v>
       </c>
       <c r="C11" t="s">
@@ -926,7 +936,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
+      <c r="A12" s="9"/>
       <c r="C12" t="s">
         <v>24</v>
       </c>
@@ -962,7 +972,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
+      <c r="A13" s="9"/>
       <c r="B13" t="s">
         <v>21</v>
       </c>
@@ -1001,7 +1011,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="8"/>
+      <c r="A14" s="9"/>
       <c r="C14" t="s">
         <v>24</v>
       </c>
@@ -1037,7 +1047,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
+      <c r="A15" s="9"/>
       <c r="C15" t="s">
         <v>24</v>
       </c>
@@ -1073,7 +1083,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
+      <c r="A16" s="9"/>
       <c r="C16" t="s">
         <v>44</v>
       </c>
@@ -1109,7 +1119,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="8"/>
+      <c r="A17" s="9"/>
       <c r="C17" t="s">
         <v>43</v>
       </c>
@@ -1145,7 +1155,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="8"/>
+      <c r="A18" s="9"/>
       <c r="C18" t="s">
         <v>45</v>
       </c>
@@ -1181,7 +1191,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C19" t="s">
@@ -1219,7 +1229,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
+      <c r="A20" s="8"/>
       <c r="C20" t="s">
         <v>24</v>
       </c>
@@ -1255,7 +1265,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C21" t="s">
@@ -1293,7 +1303,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
+      <c r="A22" s="8"/>
       <c r="C22" t="s">
         <v>47</v>
       </c>
@@ -1329,7 +1339,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="7"/>
+      <c r="A23" s="8"/>
       <c r="C23" t="s">
         <v>48</v>
       </c>
@@ -1365,7 +1375,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" s="7"/>
+      <c r="A24" s="8"/>
       <c r="C24" t="s">
         <v>49</v>
       </c>
@@ -1401,7 +1411,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="8" t="s">
         <v>63</v>
       </c>
       <c r="C25" s="6" t="s">
@@ -1415,7 +1425,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="7"/>
+      <c r="A26" s="8"/>
       <c r="C26" s="6" t="s">
         <v>66</v>
       </c>
@@ -1434,7 +1444,10 @@
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="7"/>
+      <c r="A27" s="8"/>
+      <c r="C27" s="7" t="s">
+        <v>72</v>
+      </c>
       <c r="D27" t="s">
         <v>68</v>
       </c>
@@ -1450,71 +1463,81 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="D28" t="s">
         <v>70</v>
       </c>
       <c r="F28">
         <v>3</v>
       </c>
-      <c r="K28" s="10" t="s">
+      <c r="K28" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
       <c r="N28">
         <v>76.52</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29" s="8"/>
+      <c r="C29" s="7" t="s">
+        <v>74</v>
+      </c>
       <c r="D29" t="s">
         <v>71</v>
       </c>
       <c r="F29">
         <v>2</v>
       </c>
-      <c r="K29" s="10" t="s">
+      <c r="K29" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
       <c r="N29">
         <v>174</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="K30" s="10" t="s">
+      <c r="K30" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
       <c r="N30">
         <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="K31" s="10" t="s">
+      <c r="K31" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="L31" s="10"/>
-      <c r="M31" s="10"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
       <c r="N31">
         <f>N29-N30</f>
         <v>124</v>
       </c>
     </row>
     <row r="33" spans="11:14" x14ac:dyDescent="0.3">
-      <c r="K33" s="9" t="s">
+      <c r="K33" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="L33" s="9"/>
-      <c r="M33" s="9"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
       <c r="N33">
         <f>L27+N28+N31</f>
         <v>270.84719999999999</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="A5:A10"/>
     <mergeCell ref="A11:A18"/>
@@ -1526,6 +1549,7 @@
     <mergeCell ref="K30:M30"/>
     <mergeCell ref="K31:M31"/>
     <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A28:A29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>